<commit_message>
Grosse grosse mise a jour
</commit_message>
<xml_diff>
--- a/ameliorations.xlsx
+++ b/ameliorations.xlsx
@@ -459,14 +459,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" hidden="1" customWidth="1"/>
@@ -532,18 +532,18 @@
       </c>
       <c r="B3" s="1">
         <f>B2+C3</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <f>C2+D3</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <f>D2+E3</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>8</v>
@@ -561,15 +561,15 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B52" si="0">B3+C4</f>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ref="C4:C52" si="1">C3+D4</f>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ref="D4:D52" si="2">D3+E4</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -590,15 +590,15 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -619,15 +619,15 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -648,15 +648,15 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -677,15 +677,15 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>249</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -706,15 +706,15 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>206</v>
+        <v>346</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -735,15 +735,15 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>284</v>
+        <v>464</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -764,15 +764,15 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>380</v>
+        <v>605</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -794,15 +794,15 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>498</v>
+        <v>773</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>168</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1">
         <v>4</v>
@@ -815,15 +815,15 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>642</v>
+        <v>972</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>199</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E13" s="1">
         <v>4</v>
@@ -836,15 +836,15 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>816</v>
+        <v>1206</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>174</v>
+        <v>234</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1">
         <v>4</v>
@@ -857,15 +857,15 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>1024</v>
+        <v>1479</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>273</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E15" s="1">
         <v>4</v>
@@ -878,15 +878,15 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>1270</v>
+        <v>1795</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>246</v>
+        <v>316</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E16" s="1">
         <v>4</v>
@@ -899,15 +899,15 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>1560</v>
+        <v>2160</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>290</v>
+        <v>365</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E17" s="1">
         <v>6</v>
@@ -920,15 +920,15 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>1900</v>
+        <v>2580</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>340</v>
+        <v>420</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E18" s="1">
         <v>6</v>
@@ -941,15 +941,15 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>2296</v>
+        <v>3061</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>396</v>
+        <v>481</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="2"/>
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E19" s="1">
         <v>6</v>
@@ -962,15 +962,15 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>2754</v>
+        <v>3609</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="1"/>
-        <v>458</v>
+        <v>548</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E20" s="1">
         <v>6</v>
@@ -983,15 +983,15 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>3280</v>
+        <v>4230</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="1"/>
-        <v>526</v>
+        <v>621</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="2"/>
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1">
         <v>6</v>
@@ -1004,15 +1004,15 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>3882</v>
+        <v>4932</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="1"/>
-        <v>602</v>
+        <v>702</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E22" s="1">
         <v>8</v>
@@ -1025,15 +1025,15 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>4568</v>
+        <v>5723</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="1"/>
-        <v>686</v>
+        <v>791</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E23" s="1">
         <v>8</v>
@@ -1046,15 +1046,15 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>5346</v>
+        <v>6611</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="1"/>
-        <v>778</v>
+        <v>888</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="2"/>
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E24" s="1">
         <v>8</v>
@@ -1067,15 +1067,15 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>6224</v>
+        <v>7604</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="1"/>
-        <v>878</v>
+        <v>993</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E25" s="1">
         <v>8</v>
@@ -1088,15 +1088,15 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" si="0"/>
-        <v>7210</v>
+        <v>8710</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>986</v>
+        <v>1106</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="2"/>
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E26" s="1">
         <v>8</v>
@@ -1109,15 +1109,15 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
-        <v>8314</v>
+        <v>9939</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="1"/>
-        <v>1104</v>
+        <v>1229</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="2"/>
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E27" s="1">
         <v>10</v>
@@ -1130,15 +1130,15 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>9546</v>
+        <v>11301</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="1"/>
-        <v>1232</v>
+        <v>1362</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="2"/>
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E28" s="1">
         <v>10</v>
@@ -1151,15 +1151,15 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>10916</v>
+        <v>12806</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="1"/>
-        <v>1370</v>
+        <v>1505</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="2"/>
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E29" s="1">
         <v>10</v>
@@ -1172,15 +1172,15 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>12434</v>
+        <v>14464</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>1518</v>
+        <v>1658</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="2"/>
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="E30" s="1">
         <v>10</v>
@@ -1193,15 +1193,15 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" si="0"/>
-        <v>14110</v>
+        <v>16285</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="1"/>
-        <v>1676</v>
+        <v>1821</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="2"/>
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E31" s="1">
         <v>10</v>
@@ -1214,15 +1214,15 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>
-        <v>15956</v>
+        <v>18281</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="1"/>
-        <v>1846</v>
+        <v>1996</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="2"/>
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E32" s="1">
         <v>12</v>
@@ -1235,15 +1235,15 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" si="0"/>
-        <v>17984</v>
+        <v>20464</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="1"/>
-        <v>2028</v>
+        <v>2183</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="2"/>
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E33" s="1">
         <v>12</v>
@@ -1256,15 +1256,15 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" si="0"/>
-        <v>20206</v>
+        <v>22846</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="1"/>
-        <v>2222</v>
+        <v>2382</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="2"/>
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E34" s="1">
         <v>12</v>
@@ -1277,15 +1277,15 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" si="0"/>
-        <v>22634</v>
+        <v>25439</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="1"/>
-        <v>2428</v>
+        <v>2593</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="2"/>
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E35" s="1">
         <v>12</v>
@@ -1298,15 +1298,15 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" si="0"/>
-        <v>25280</v>
+        <v>28255</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="1"/>
-        <v>2646</v>
+        <v>2816</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" si="2"/>
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="E36" s="1">
         <v>12</v>
@@ -1319,15 +1319,15 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" si="0"/>
-        <v>28158</v>
+        <v>31308</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" si="1"/>
-        <v>2878</v>
+        <v>3053</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" si="2"/>
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E37" s="1">
         <v>14</v>
@@ -1340,15 +1340,15 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" si="0"/>
-        <v>31282</v>
+        <v>34612</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="1"/>
-        <v>3124</v>
+        <v>3304</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" si="2"/>
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E38" s="1">
         <v>14</v>
@@ -1361,15 +1361,15 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" si="0"/>
-        <v>34666</v>
+        <v>38181</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" si="1"/>
-        <v>3384</v>
+        <v>3569</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" si="2"/>
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="E39" s="1">
         <v>14</v>
@@ -1382,15 +1382,15 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" si="0"/>
-        <v>38324</v>
+        <v>42029</v>
       </c>
       <c r="C40" s="1">
         <f t="shared" si="1"/>
-        <v>3658</v>
+        <v>3848</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" si="2"/>
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="E40" s="1">
         <v>14</v>
@@ -1403,15 +1403,15 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" si="0"/>
-        <v>42270</v>
+        <v>46170</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" si="1"/>
-        <v>3946</v>
+        <v>4141</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" si="2"/>
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="E41" s="1">
         <v>14</v>
@@ -1424,15 +1424,15 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" si="0"/>
-        <v>46520</v>
+        <v>50620</v>
       </c>
       <c r="C42" s="1">
         <f t="shared" si="1"/>
-        <v>4250</v>
+        <v>4450</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" si="2"/>
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="E42" s="1">
         <v>16</v>
@@ -1445,15 +1445,15 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" si="0"/>
-        <v>51090</v>
+        <v>55395</v>
       </c>
       <c r="C43" s="1">
         <f t="shared" si="1"/>
-        <v>4570</v>
+        <v>4775</v>
       </c>
       <c r="D43" s="1">
         <f t="shared" si="2"/>
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="E43" s="1">
         <v>16</v>
@@ -1466,15 +1466,15 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" si="0"/>
-        <v>55996</v>
+        <v>60511</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" si="1"/>
-        <v>4906</v>
+        <v>5116</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" si="2"/>
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="E44" s="1">
         <v>16</v>
@@ -1487,15 +1487,15 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" si="0"/>
-        <v>61254</v>
+        <v>65984</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" si="1"/>
-        <v>5258</v>
+        <v>5473</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" si="2"/>
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="E45" s="1">
         <v>16</v>
@@ -1508,15 +1508,15 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" si="0"/>
-        <v>66880</v>
+        <v>71830</v>
       </c>
       <c r="C46" s="1">
         <f t="shared" si="1"/>
-        <v>5626</v>
+        <v>5846</v>
       </c>
       <c r="D46" s="1">
         <f t="shared" si="2"/>
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="E46" s="1">
         <v>16</v>
@@ -1529,15 +1529,15 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" si="0"/>
-        <v>72892</v>
+        <v>78067</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" si="1"/>
-        <v>6012</v>
+        <v>6237</v>
       </c>
       <c r="D47" s="1">
         <f t="shared" si="2"/>
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="E47" s="1">
         <v>18</v>
@@ -1550,15 +1550,15 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" si="0"/>
-        <v>79308</v>
+        <v>84713</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" si="1"/>
-        <v>6416</v>
+        <v>6646</v>
       </c>
       <c r="D48" s="1">
         <f t="shared" si="2"/>
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="E48" s="1">
         <v>18</v>
@@ -1571,15 +1571,15 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" si="0"/>
-        <v>86146</v>
+        <v>91786</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" si="1"/>
-        <v>6838</v>
+        <v>7073</v>
       </c>
       <c r="D49" s="1">
         <f t="shared" si="2"/>
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="E49" s="1">
         <v>18</v>
@@ -1592,15 +1592,15 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" si="0"/>
-        <v>93424</v>
+        <v>99304</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" si="1"/>
-        <v>7278</v>
+        <v>7518</v>
       </c>
       <c r="D50" s="1">
         <f t="shared" si="2"/>
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="E50" s="1">
         <v>18</v>
@@ -1613,15 +1613,15 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" si="0"/>
-        <v>101160</v>
+        <v>107285</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" si="1"/>
-        <v>7736</v>
+        <v>7981</v>
       </c>
       <c r="D51" s="1">
         <f t="shared" si="2"/>
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="E51" s="1">
         <v>18</v>
@@ -1634,15 +1634,15 @@
       </c>
       <c r="B52" s="1">
         <f t="shared" si="0"/>
-        <v>109374</v>
+        <v>115749</v>
       </c>
       <c r="C52" s="1">
         <f t="shared" si="1"/>
-        <v>8214</v>
+        <v>8464</v>
       </c>
       <c r="D52" s="1">
         <f t="shared" si="2"/>
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="E52" s="1">
         <v>20</v>
@@ -1655,15 +1655,15 @@
       </c>
       <c r="B53" s="1">
         <f t="shared" ref="B53:B102" si="5">B52+C53</f>
-        <v>118086</v>
+        <v>124716</v>
       </c>
       <c r="C53" s="1">
         <f t="shared" ref="C53:C102" si="6">C52+D53</f>
-        <v>8712</v>
+        <v>8967</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" ref="D53:D102" si="7">D52+E53</f>
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="E53" s="1">
         <v>20</v>
@@ -1676,15 +1676,15 @@
       </c>
       <c r="B54" s="1">
         <f t="shared" si="5"/>
-        <v>127316</v>
+        <v>134206</v>
       </c>
       <c r="C54" s="1">
         <f t="shared" si="6"/>
-        <v>9230</v>
+        <v>9490</v>
       </c>
       <c r="D54" s="1">
         <f t="shared" si="7"/>
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="E54" s="1">
         <v>20</v>
@@ -1697,15 +1697,15 @@
       </c>
       <c r="B55" s="1">
         <f t="shared" si="5"/>
-        <v>137084</v>
+        <v>144239</v>
       </c>
       <c r="C55" s="1">
         <f t="shared" si="6"/>
-        <v>9768</v>
+        <v>10033</v>
       </c>
       <c r="D55" s="1">
         <f t="shared" si="7"/>
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="E55" s="1">
         <v>20</v>
@@ -1718,15 +1718,15 @@
       </c>
       <c r="B56" s="1">
         <f t="shared" si="5"/>
-        <v>147410</v>
+        <v>154835</v>
       </c>
       <c r="C56" s="1">
         <f t="shared" si="6"/>
-        <v>10326</v>
+        <v>10596</v>
       </c>
       <c r="D56" s="1">
         <f t="shared" si="7"/>
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="E56" s="1">
         <v>20</v>
@@ -1739,15 +1739,15 @@
       </c>
       <c r="B57" s="1">
         <f t="shared" si="5"/>
-        <v>158316</v>
+        <v>166016</v>
       </c>
       <c r="C57" s="1">
         <f t="shared" si="6"/>
-        <v>10906</v>
+        <v>11181</v>
       </c>
       <c r="D57" s="1">
         <f t="shared" si="7"/>
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="E57" s="1">
         <v>22</v>
@@ -1760,15 +1760,15 @@
       </c>
       <c r="B58" s="1">
         <f t="shared" si="5"/>
-        <v>169824</v>
+        <v>177804</v>
       </c>
       <c r="C58" s="1">
         <f t="shared" si="6"/>
-        <v>11508</v>
+        <v>11788</v>
       </c>
       <c r="D58" s="1">
         <f t="shared" si="7"/>
-        <v>602</v>
+        <v>607</v>
       </c>
       <c r="E58" s="1">
         <v>22</v>
@@ -1781,15 +1781,15 @@
       </c>
       <c r="B59" s="1">
         <f t="shared" si="5"/>
-        <v>181956</v>
+        <v>190221</v>
       </c>
       <c r="C59" s="1">
         <f t="shared" si="6"/>
-        <v>12132</v>
+        <v>12417</v>
       </c>
       <c r="D59" s="1">
         <f t="shared" si="7"/>
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="E59" s="1">
         <v>22</v>
@@ -1802,15 +1802,15 @@
       </c>
       <c r="B60" s="1">
         <f t="shared" si="5"/>
-        <v>194734</v>
+        <v>203289</v>
       </c>
       <c r="C60" s="1">
         <f t="shared" si="6"/>
-        <v>12778</v>
+        <v>13068</v>
       </c>
       <c r="D60" s="1">
         <f t="shared" si="7"/>
-        <v>646</v>
+        <v>651</v>
       </c>
       <c r="E60" s="1">
         <v>22</v>
@@ -1823,15 +1823,15 @@
       </c>
       <c r="B61" s="1">
         <f t="shared" si="5"/>
-        <v>208180</v>
+        <v>217030</v>
       </c>
       <c r="C61" s="1">
         <f t="shared" si="6"/>
-        <v>13446</v>
+        <v>13741</v>
       </c>
       <c r="D61" s="1">
         <f t="shared" si="7"/>
-        <v>668</v>
+        <v>673</v>
       </c>
       <c r="E61" s="1">
         <v>22</v>
@@ -1844,15 +1844,15 @@
       </c>
       <c r="B62" s="1">
         <f t="shared" si="5"/>
-        <v>222318</v>
+        <v>231468</v>
       </c>
       <c r="C62" s="1">
         <f t="shared" si="6"/>
-        <v>14138</v>
+        <v>14438</v>
       </c>
       <c r="D62" s="1">
         <f t="shared" si="7"/>
-        <v>692</v>
+        <v>697</v>
       </c>
       <c r="E62" s="1">
         <v>24</v>
@@ -1865,15 +1865,15 @@
       </c>
       <c r="B63" s="1">
         <f t="shared" si="5"/>
-        <v>237172</v>
+        <v>246627</v>
       </c>
       <c r="C63" s="1">
         <f t="shared" si="6"/>
-        <v>14854</v>
+        <v>15159</v>
       </c>
       <c r="D63" s="1">
         <f t="shared" si="7"/>
-        <v>716</v>
+        <v>721</v>
       </c>
       <c r="E63" s="1">
         <v>24</v>
@@ -1886,15 +1886,15 @@
       </c>
       <c r="B64" s="1">
         <f t="shared" si="5"/>
-        <v>252766</v>
+        <v>262531</v>
       </c>
       <c r="C64" s="1">
         <f t="shared" si="6"/>
-        <v>15594</v>
+        <v>15904</v>
       </c>
       <c r="D64" s="1">
         <f t="shared" si="7"/>
-        <v>740</v>
+        <v>745</v>
       </c>
       <c r="E64" s="1">
         <v>24</v>
@@ -1907,15 +1907,15 @@
       </c>
       <c r="B65" s="1">
         <f t="shared" si="5"/>
-        <v>269124</v>
+        <v>279204</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" si="6"/>
-        <v>16358</v>
+        <v>16673</v>
       </c>
       <c r="D65" s="1">
         <f t="shared" si="7"/>
-        <v>764</v>
+        <v>769</v>
       </c>
       <c r="E65" s="1">
         <v>24</v>
@@ -1928,15 +1928,15 @@
       </c>
       <c r="B66" s="1">
         <f t="shared" si="5"/>
-        <v>286270</v>
+        <v>296670</v>
       </c>
       <c r="C66" s="1">
         <f t="shared" si="6"/>
-        <v>17146</v>
+        <v>17466</v>
       </c>
       <c r="D66" s="1">
         <f t="shared" si="7"/>
-        <v>788</v>
+        <v>793</v>
       </c>
       <c r="E66" s="1">
         <v>24</v>
@@ -1949,15 +1949,15 @@
       </c>
       <c r="B67" s="1">
         <f t="shared" si="5"/>
-        <v>304230</v>
+        <v>314955</v>
       </c>
       <c r="C67" s="1">
         <f t="shared" si="6"/>
-        <v>17960</v>
+        <v>18285</v>
       </c>
       <c r="D67" s="1">
         <f t="shared" si="7"/>
-        <v>814</v>
+        <v>819</v>
       </c>
       <c r="E67" s="1">
         <v>26</v>
@@ -1970,15 +1970,15 @@
       </c>
       <c r="B68" s="1">
         <f t="shared" si="5"/>
-        <v>323030</v>
+        <v>334085</v>
       </c>
       <c r="C68" s="1">
         <f t="shared" si="6"/>
-        <v>18800</v>
+        <v>19130</v>
       </c>
       <c r="D68" s="1">
         <f t="shared" si="7"/>
-        <v>840</v>
+        <v>845</v>
       </c>
       <c r="E68" s="1">
         <v>26</v>
@@ -1991,15 +1991,15 @@
       </c>
       <c r="B69" s="1">
         <f t="shared" si="5"/>
-        <v>342696</v>
+        <v>354086</v>
       </c>
       <c r="C69" s="1">
         <f t="shared" si="6"/>
-        <v>19666</v>
+        <v>20001</v>
       </c>
       <c r="D69" s="1">
         <f t="shared" si="7"/>
-        <v>866</v>
+        <v>871</v>
       </c>
       <c r="E69" s="1">
         <v>26</v>
@@ -2012,15 +2012,15 @@
       </c>
       <c r="B70" s="1">
         <f t="shared" si="5"/>
-        <v>363254</v>
+        <v>374984</v>
       </c>
       <c r="C70" s="1">
         <f t="shared" si="6"/>
-        <v>20558</v>
+        <v>20898</v>
       </c>
       <c r="D70" s="1">
         <f t="shared" si="7"/>
-        <v>892</v>
+        <v>897</v>
       </c>
       <c r="E70" s="1">
         <v>26</v>
@@ -2033,15 +2033,15 @@
       </c>
       <c r="B71" s="1">
         <f t="shared" si="5"/>
-        <v>384730</v>
+        <v>396805</v>
       </c>
       <c r="C71" s="1">
         <f t="shared" si="6"/>
-        <v>21476</v>
+        <v>21821</v>
       </c>
       <c r="D71" s="1">
         <f t="shared" si="7"/>
-        <v>918</v>
+        <v>923</v>
       </c>
       <c r="E71" s="1">
         <v>26</v>
@@ -2054,15 +2054,15 @@
       </c>
       <c r="B72" s="1">
         <f t="shared" si="5"/>
-        <v>407152</v>
+        <v>419577</v>
       </c>
       <c r="C72" s="1">
         <f t="shared" si="6"/>
-        <v>22422</v>
+        <v>22772</v>
       </c>
       <c r="D72" s="1">
         <f t="shared" si="7"/>
-        <v>946</v>
+        <v>951</v>
       </c>
       <c r="E72" s="1">
         <v>28</v>
@@ -2075,15 +2075,15 @@
       </c>
       <c r="B73" s="1">
         <f t="shared" si="5"/>
-        <v>430548</v>
+        <v>443328</v>
       </c>
       <c r="C73" s="1">
-        <f t="shared" si="6"/>
-        <v>23396</v>
+        <f>C72+D73</f>
+        <v>23751</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" si="7"/>
-        <v>974</v>
+        <v>979</v>
       </c>
       <c r="E73" s="1">
         <v>28</v>
@@ -2096,15 +2096,15 @@
       </c>
       <c r="B74" s="1">
         <f t="shared" si="5"/>
-        <v>454946</v>
+        <v>468086</v>
       </c>
       <c r="C74" s="1">
         <f t="shared" si="6"/>
-        <v>24398</v>
+        <v>24758</v>
       </c>
       <c r="D74" s="1">
         <f t="shared" si="7"/>
-        <v>1002</v>
+        <v>1007</v>
       </c>
       <c r="E74" s="1">
         <v>28</v>
@@ -2117,15 +2117,15 @@
       </c>
       <c r="B75" s="1">
         <f t="shared" si="5"/>
-        <v>480374</v>
+        <v>493879</v>
       </c>
       <c r="C75" s="1">
         <f t="shared" si="6"/>
-        <v>25428</v>
+        <v>25793</v>
       </c>
       <c r="D75" s="1">
         <f t="shared" si="7"/>
-        <v>1030</v>
+        <v>1035</v>
       </c>
       <c r="E75" s="1">
         <v>28</v>
@@ -2138,15 +2138,15 @@
       </c>
       <c r="B76" s="1">
         <f t="shared" si="5"/>
-        <v>506860</v>
+        <v>520735</v>
       </c>
       <c r="C76" s="1">
         <f t="shared" si="6"/>
-        <v>26486</v>
+        <v>26856</v>
       </c>
       <c r="D76" s="1">
         <f t="shared" si="7"/>
-        <v>1058</v>
+        <v>1063</v>
       </c>
       <c r="E76" s="1">
         <v>28</v>
@@ -2159,15 +2159,15 @@
       </c>
       <c r="B77" s="1">
         <f t="shared" si="5"/>
-        <v>534434</v>
+        <v>548684</v>
       </c>
       <c r="C77" s="1">
         <f t="shared" si="6"/>
-        <v>27574</v>
+        <v>27949</v>
       </c>
       <c r="D77" s="1">
         <f t="shared" si="7"/>
-        <v>1088</v>
+        <v>1093</v>
       </c>
       <c r="E77" s="1">
         <v>30</v>
@@ -2180,15 +2180,15 @@
       </c>
       <c r="B78" s="1">
         <f t="shared" si="5"/>
-        <v>563126</v>
+        <v>577756</v>
       </c>
       <c r="C78" s="1">
         <f t="shared" si="6"/>
-        <v>28692</v>
+        <v>29072</v>
       </c>
       <c r="D78" s="1">
         <f t="shared" si="7"/>
-        <v>1118</v>
+        <v>1123</v>
       </c>
       <c r="E78" s="1">
         <v>30</v>
@@ -2201,15 +2201,15 @@
       </c>
       <c r="B79" s="1">
         <f t="shared" si="5"/>
-        <v>592966</v>
+        <v>607981</v>
       </c>
       <c r="C79" s="1">
         <f t="shared" si="6"/>
-        <v>29840</v>
+        <v>30225</v>
       </c>
       <c r="D79" s="1">
         <f t="shared" si="7"/>
-        <v>1148</v>
+        <v>1153</v>
       </c>
       <c r="E79" s="1">
         <v>30</v>
@@ -2222,15 +2222,15 @@
       </c>
       <c r="B80" s="1">
         <f t="shared" si="5"/>
-        <v>623984</v>
+        <v>639389</v>
       </c>
       <c r="C80" s="1">
         <f t="shared" si="6"/>
-        <v>31018</v>
+        <v>31408</v>
       </c>
       <c r="D80" s="1">
         <f t="shared" si="7"/>
-        <v>1178</v>
+        <v>1183</v>
       </c>
       <c r="E80" s="1">
         <v>30</v>
@@ -2243,15 +2243,15 @@
       </c>
       <c r="B81" s="1">
         <f t="shared" si="5"/>
-        <v>656210</v>
+        <v>672010</v>
       </c>
       <c r="C81" s="1">
         <f t="shared" si="6"/>
-        <v>32226</v>
+        <v>32621</v>
       </c>
       <c r="D81" s="1">
         <f t="shared" si="7"/>
-        <v>1208</v>
+        <v>1213</v>
       </c>
       <c r="E81" s="1">
         <v>30</v>
@@ -2264,15 +2264,15 @@
       </c>
       <c r="B82" s="1">
         <f t="shared" si="5"/>
-        <v>689676</v>
+        <v>705876</v>
       </c>
       <c r="C82" s="1">
         <f t="shared" si="6"/>
-        <v>33466</v>
+        <v>33866</v>
       </c>
       <c r="D82" s="1">
         <f t="shared" si="7"/>
-        <v>1240</v>
+        <v>1245</v>
       </c>
       <c r="E82" s="1">
         <v>32</v>
@@ -2285,15 +2285,15 @@
       </c>
       <c r="B83" s="1">
         <f t="shared" si="5"/>
-        <v>724414</v>
+        <v>741019</v>
       </c>
       <c r="C83" s="1">
         <f t="shared" si="6"/>
-        <v>34738</v>
+        <v>35143</v>
       </c>
       <c r="D83" s="1">
         <f t="shared" si="7"/>
-        <v>1272</v>
+        <v>1277</v>
       </c>
       <c r="E83" s="1">
         <v>32</v>
@@ -2306,15 +2306,15 @@
       </c>
       <c r="B84" s="1">
         <f t="shared" si="5"/>
-        <v>760456</v>
+        <v>777471</v>
       </c>
       <c r="C84" s="1">
         <f t="shared" si="6"/>
-        <v>36042</v>
+        <v>36452</v>
       </c>
       <c r="D84" s="1">
         <f t="shared" si="7"/>
-        <v>1304</v>
+        <v>1309</v>
       </c>
       <c r="E84" s="1">
         <v>32</v>
@@ -2327,15 +2327,15 @@
       </c>
       <c r="B85" s="1">
         <f t="shared" si="5"/>
-        <v>797834</v>
+        <v>815264</v>
       </c>
       <c r="C85" s="1">
         <f t="shared" si="6"/>
-        <v>37378</v>
+        <v>37793</v>
       </c>
       <c r="D85" s="1">
         <f t="shared" si="7"/>
-        <v>1336</v>
+        <v>1341</v>
       </c>
       <c r="E85" s="1">
         <v>32</v>
@@ -2348,15 +2348,15 @@
       </c>
       <c r="B86" s="1">
         <f t="shared" si="5"/>
-        <v>836580</v>
+        <v>854430</v>
       </c>
       <c r="C86" s="1">
         <f t="shared" si="6"/>
-        <v>38746</v>
+        <v>39166</v>
       </c>
       <c r="D86" s="1">
         <f t="shared" si="7"/>
-        <v>1368</v>
+        <v>1373</v>
       </c>
       <c r="E86" s="1">
         <v>32</v>
@@ -2369,15 +2369,15 @@
       </c>
       <c r="B87" s="1">
         <f t="shared" si="5"/>
-        <v>876728</v>
+        <v>895003</v>
       </c>
       <c r="C87" s="1">
         <f t="shared" si="6"/>
-        <v>40148</v>
+        <v>40573</v>
       </c>
       <c r="D87" s="1">
         <f t="shared" si="7"/>
-        <v>1402</v>
+        <v>1407</v>
       </c>
       <c r="E87" s="1">
         <v>34</v>
@@ -2390,15 +2390,15 @@
       </c>
       <c r="B88" s="1">
         <f t="shared" si="5"/>
-        <v>918312</v>
+        <v>937017</v>
       </c>
       <c r="C88" s="1">
         <f t="shared" si="6"/>
-        <v>41584</v>
+        <v>42014</v>
       </c>
       <c r="D88" s="1">
         <f t="shared" si="7"/>
-        <v>1436</v>
+        <v>1441</v>
       </c>
       <c r="E88" s="1">
         <v>34</v>
@@ -2411,15 +2411,15 @@
       </c>
       <c r="B89" s="1">
         <f t="shared" si="5"/>
-        <v>961366</v>
+        <v>980506</v>
       </c>
       <c r="C89" s="1">
         <f t="shared" si="6"/>
-        <v>43054</v>
+        <v>43489</v>
       </c>
       <c r="D89" s="1">
         <f t="shared" si="7"/>
-        <v>1470</v>
+        <v>1475</v>
       </c>
       <c r="E89" s="1">
         <v>34</v>
@@ -2432,15 +2432,15 @@
       </c>
       <c r="B90" s="1">
         <f t="shared" si="5"/>
-        <v>1005924</v>
+        <v>1025504</v>
       </c>
       <c r="C90" s="1">
         <f t="shared" si="6"/>
-        <v>44558</v>
+        <v>44998</v>
       </c>
       <c r="D90" s="1">
         <f t="shared" si="7"/>
-        <v>1504</v>
+        <v>1509</v>
       </c>
       <c r="E90" s="1">
         <v>34</v>
@@ -2453,15 +2453,15 @@
       </c>
       <c r="B91" s="1">
         <f t="shared" si="5"/>
-        <v>1052020</v>
+        <v>1072045</v>
       </c>
       <c r="C91" s="1">
         <f t="shared" si="6"/>
-        <v>46096</v>
+        <v>46541</v>
       </c>
       <c r="D91" s="1">
         <f t="shared" si="7"/>
-        <v>1538</v>
+        <v>1543</v>
       </c>
       <c r="E91" s="1">
         <v>34</v>
@@ -2474,15 +2474,15 @@
       </c>
       <c r="B92" s="1">
         <f t="shared" si="5"/>
-        <v>1099690</v>
+        <v>1120165</v>
       </c>
       <c r="C92" s="1">
         <f t="shared" si="6"/>
-        <v>47670</v>
+        <v>48120</v>
       </c>
       <c r="D92" s="1">
         <f t="shared" si="7"/>
-        <v>1574</v>
+        <v>1579</v>
       </c>
       <c r="E92" s="1">
         <v>36</v>
@@ -2495,15 +2495,15 @@
       </c>
       <c r="B93" s="1">
         <f t="shared" si="5"/>
-        <v>1148970</v>
+        <v>1169900</v>
       </c>
       <c r="C93" s="1">
         <f t="shared" si="6"/>
-        <v>49280</v>
+        <v>49735</v>
       </c>
       <c r="D93" s="1">
         <f t="shared" si="7"/>
-        <v>1610</v>
+        <v>1615</v>
       </c>
       <c r="E93" s="1">
         <v>36</v>
@@ -2516,15 +2516,15 @@
       </c>
       <c r="B94" s="1">
         <f t="shared" si="5"/>
-        <v>1199896</v>
+        <v>1221286</v>
       </c>
       <c r="C94" s="1">
         <f t="shared" si="6"/>
-        <v>50926</v>
+        <v>51386</v>
       </c>
       <c r="D94" s="1">
         <f t="shared" si="7"/>
-        <v>1646</v>
+        <v>1651</v>
       </c>
       <c r="E94" s="1">
         <v>36</v>
@@ -2537,15 +2537,15 @@
       </c>
       <c r="B95" s="1">
         <f t="shared" si="5"/>
-        <v>1252504</v>
+        <v>1274359</v>
       </c>
       <c r="C95" s="1">
         <f t="shared" si="6"/>
-        <v>52608</v>
+        <v>53073</v>
       </c>
       <c r="D95" s="1">
         <f t="shared" si="7"/>
-        <v>1682</v>
+        <v>1687</v>
       </c>
       <c r="E95" s="1">
         <v>36</v>
@@ -2558,15 +2558,15 @@
       </c>
       <c r="B96" s="1">
         <f t="shared" si="5"/>
-        <v>1306830</v>
+        <v>1329155</v>
       </c>
       <c r="C96" s="1">
         <f t="shared" si="6"/>
-        <v>54326</v>
+        <v>54796</v>
       </c>
       <c r="D96" s="1">
         <f t="shared" si="7"/>
-        <v>1718</v>
+        <v>1723</v>
       </c>
       <c r="E96" s="1">
         <v>36</v>
@@ -2579,15 +2579,15 @@
       </c>
       <c r="B97" s="1">
         <f t="shared" si="5"/>
-        <v>1362912</v>
+        <v>1385712</v>
       </c>
       <c r="C97" s="1">
         <f t="shared" si="6"/>
-        <v>56082</v>
+        <v>56557</v>
       </c>
       <c r="D97" s="1">
         <f t="shared" si="7"/>
-        <v>1756</v>
+        <v>1761</v>
       </c>
       <c r="E97" s="1">
         <v>38</v>
@@ -2600,15 +2600,15 @@
       </c>
       <c r="B98" s="1">
         <f t="shared" si="5"/>
-        <v>1420788</v>
+        <v>1444068</v>
       </c>
       <c r="C98" s="1">
         <f t="shared" si="6"/>
-        <v>57876</v>
+        <v>58356</v>
       </c>
       <c r="D98" s="1">
         <f t="shared" si="7"/>
-        <v>1794</v>
+        <v>1799</v>
       </c>
       <c r="E98" s="1">
         <v>38</v>
@@ -2621,15 +2621,15 @@
       </c>
       <c r="B99" s="1">
         <f t="shared" si="5"/>
-        <v>1480496</v>
+        <v>1504261</v>
       </c>
       <c r="C99" s="1">
         <f t="shared" si="6"/>
-        <v>59708</v>
+        <v>60193</v>
       </c>
       <c r="D99" s="1">
         <f t="shared" si="7"/>
-        <v>1832</v>
+        <v>1837</v>
       </c>
       <c r="E99" s="1">
         <v>38</v>
@@ -2642,15 +2642,15 @@
       </c>
       <c r="B100" s="1">
         <f t="shared" si="5"/>
-        <v>1542074</v>
+        <v>1566329</v>
       </c>
       <c r="C100" s="1">
         <f t="shared" si="6"/>
-        <v>61578</v>
+        <v>62068</v>
       </c>
       <c r="D100" s="1">
         <f t="shared" si="7"/>
-        <v>1870</v>
+        <v>1875</v>
       </c>
       <c r="E100" s="1">
         <v>38</v>
@@ -2663,15 +2663,15 @@
       </c>
       <c r="B101" s="1">
         <f t="shared" si="5"/>
-        <v>1605560</v>
+        <v>1630310</v>
       </c>
       <c r="C101" s="1">
         <f t="shared" si="6"/>
-        <v>63486</v>
+        <v>63981</v>
       </c>
       <c r="D101" s="1">
         <f t="shared" si="7"/>
-        <v>1908</v>
+        <v>1913</v>
       </c>
       <c r="E101" s="1">
         <v>38</v>
@@ -2684,15 +2684,15 @@
       </c>
       <c r="B102" s="1">
         <f t="shared" si="5"/>
-        <v>1670994</v>
+        <v>1696244</v>
       </c>
       <c r="C102" s="1">
         <f t="shared" si="6"/>
-        <v>65434</v>
+        <v>65934</v>
       </c>
       <c r="D102" s="1">
         <f t="shared" si="7"/>
-        <v>1948</v>
+        <v>1953</v>
       </c>
       <c r="E102" s="1">
         <v>40</v>

</xml_diff>